<commit_message>
agregue el  documento edt version 2
</commit_message>
<xml_diff>
--- a/DiccionarioEDT.xlsx
+++ b/DiccionarioEDT.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdalbertoPc\Documents\11voCiclo\IngenieriaDeProyectos\Proyecto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="12915" windowHeight="4695"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Diccionario" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>ACT EDT</t>
   </si>
@@ -36,42 +39,13 @@
     <t>INICIO</t>
   </si>
   <si>
-    <t>Se realizo una reunion con el director del establecimiento para dar solucion a la problemática que se ha generado por mantener los registros fisicos del establecimiento.</t>
-  </si>
-  <si>
-    <t>DEFINICION DEL PROBLEMA</t>
-  </si>
-  <si>
-    <t>Los procesos actualmente se realizan de forma manual y los expedientes se encuentran solamente en forma física lo que dificulta la búsqueda de archivos, expedientes y llevar una buena administración.</t>
-  </si>
-  <si>
     <t>1.2</t>
   </si>
   <si>
-    <t>COORDINACIONES</t>
-  </si>
-  <si>
-    <t>Gestion para Elaboracion del acta de consitucion del proyecto, Elaboracion del plan de direccion del proyecto y elaboracion del EDT</t>
-  </si>
-  <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
-    <t>1.1.2</t>
-  </si>
-  <si>
     <t>ANALISIS</t>
   </si>
   <si>
     <t>Proceso mediante el cual definimos la informacion necesaria para abordar el proceso de diseño, comprende actividades fundamentales para el modelado de la información.</t>
-  </si>
-  <si>
-    <t>* Propuesta de Proyecto</t>
-  </si>
-  <si>
-    <t>* Acta de consitucion del proyecto
-* Plan de direccion del proyecto 
-* Estructua de Desgloce del Trabajo</t>
   </si>
   <si>
     <t>* Casos de Uso
@@ -82,13 +56,6 @@
 * Diagrama de Despliegue</t>
   </si>
   <si>
-    <t>* Entrevista con Product Owner (Cliente)</t>
-  </si>
-  <si>
-    <t>* Analista de Calidad
-* Product Owner</t>
-  </si>
-  <si>
     <t>* Analista de Calidad
 * Product Owner
 * Analista Funcional
@@ -102,6 +69,109 @@
   </si>
   <si>
     <t>Durante la fase de diseño se elaboraran los diagramas necesarios en base al analisis de la informacion realizada en el proceso 1.2, que serviran como inicio al siguiente proceso 1.4</t>
+  </si>
+  <si>
+    <t>* Analista de Calidad
+* Lider de Proyecto
+* Programador</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>PROGRAMACION</t>
+  </si>
+  <si>
+    <t>Implementacion de Diagramas para elaboracion y modelado de datos utilizando las herramientas de programacion definidas en el plan de recursos, herramientas y tecnologias de desarrollo.</t>
+  </si>
+  <si>
+    <t>* Creacion de Base de Datos
+* Creacion de Software
+* Programacion de Módulos
+* Programacion de Interfaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Programador 
+* Lider de Proyecto
+* Analista Funcional
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 </t>
+  </si>
+  <si>
+    <t>PRUEBAS</t>
+  </si>
+  <si>
+    <t>* Pruebas de GUI
+* Pruebas de Integridad de Datos y BD
+* Pruebas de Seguridad y Control de Acceso
+* Pruebas de Caja Blanca
+* Pruebas de Caja Negra 
+* Pruebas de Desempeño
+* Pruebas de Integracion
+* Pruebas de Estrés</t>
+  </si>
+  <si>
+    <t>Actividades que evaluaran la calidad, eficiencia, efectividad, operabilidad, integridad de las actividades, procesos y datos del sistema, asi como la satisfaccion del usuario.</t>
+  </si>
+  <si>
+    <t>* Lider de proyecto 
+* Analista de Calidad
+* Product Owner</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPLEMENTACION </t>
+  </si>
+  <si>
+    <t>* Instalacion de Base de Datos
+* Instalacion del Software</t>
+  </si>
+  <si>
+    <t>* Entrega de Manual de Usuario
+* Acta de Entrega
+* Terminacion del Contrato</t>
+  </si>
+  <si>
+    <t>Fase en la cual se implementara el software diseñado y desarrollado para el cliente.</t>
+  </si>
+  <si>
+    <t>* Lider de proyecto 
+* Product Owner</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>CIERRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: </t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Durante esta actividad se entregara la informacion necesaria al cliente para el uso e implementacion del sistema implementado.</t>
+  </si>
+  <si>
+    <t>* Lider del Proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICCIONARIO EDT      </t>
+  </si>
+  <si>
+    <t>Dutante este proceso se definira la informacion necesaria para la solucion del problema presentado asi como la planeacion de la ejecucion del poryecto y planes de soporte al proyecto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Acta de consitucion del proyecto
+* Plan de direccion del proyecto </t>
   </si>
   <si>
     <t>* Modelo de Software
@@ -114,110 +184,11 @@
   - Modelo Entidad Relacion
   - Diagrama de Flujo de Datos</t>
   </si>
-  <si>
-    <t>* Analista de Calidad
-* Lider de Proyecto
-* Programador</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>PROGRAMACION</t>
-  </si>
-  <si>
-    <t>Implementacion de Diagramas para elaboracion y modelado de datos utilizando las herramientas de programacion definidas en el plan de recursos, herramientas y tecnologias de desarrollo.</t>
-  </si>
-  <si>
-    <t>* Creacion de Base de Datos
-* Creacion de Software
-* Programacion de Módulos
-* Programacion de Interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Programador 
-* Lider de Proyecto
-* Analista Funcional
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5 </t>
-  </si>
-  <si>
-    <t>PRUEBAS</t>
-  </si>
-  <si>
-    <t>* Pruebas de GUI
-* Pruebas de Integridad de Datos y BD
-* Pruebas de Seguridad y Control de Acceso
-* Pruebas de Caja Blanca
-* Pruebas de Caja Negra 
-* Pruebas de Desempeño
-* Pruebas de Integracion
-* Pruebas de Estrés</t>
-  </si>
-  <si>
-    <t>Actividades que evaluaran la calidad, eficiencia, efectividad, operabilidad, integridad de las actividades, procesos y datos del sistema, asi como la satisfaccion del usuario.</t>
-  </si>
-  <si>
-    <t>* Lider de proyecto 
-* Analista de Calidad
-* Product Owner</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPLEMENTACION </t>
-  </si>
-  <si>
-    <t>* Instalacion de Base de Datos
-* Instalacion del Software</t>
-  </si>
-  <si>
-    <t>* Entrega de Manual de Usuario
-* Acta de Entrega
-* Terminacion del Contrato</t>
-  </si>
-  <si>
-    <t>Fase en la cual se implementara el software diseñado y desarrollado para el cliente.</t>
-  </si>
-  <si>
-    <t>* Lider de proyecto 
-* Product Owner</t>
-  </si>
-  <si>
-    <t>1.7</t>
-  </si>
-  <si>
-    <t>CIERRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICCIONARIO DEL EDT      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Version: </t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Durante esta actividad se entregara la informacion necesaria al cliente para el uso e implementacion del sistema implementado.</t>
-  </si>
-  <si>
-    <t>* Lider del proyecto</t>
-  </si>
-  <si>
-    <t>* Lider del Proyecto</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,61 +407,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,6 +463,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -549,7 +514,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,9 +547,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,6 +599,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -793,40 +792,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E1" s="1"/>
-    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+    <row r="3" spans="2:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2">
         <v>42450</v>
@@ -834,173 +832,139 @@
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="C9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="F12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="4" t="s">
+    </row>
+    <row r="13" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="C13" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="D13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="13" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="14" spans="2:6" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="F14" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1010,28 +974,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>